<commit_message>
final commit 2020 - condition backup
</commit_message>
<xml_diff>
--- a/Cam2calib.xlsx
+++ b/Cam2calib.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23426"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D775B8-8DE7-4212-8615-986D8A99D9AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DE68FD9-6BF4-4AC1-BBB2-BC45FDB76975}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33540" yWindow="4320" windowWidth="24686" windowHeight="13217" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13131" yWindow="4500" windowWidth="17718" windowHeight="13226" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -352,13 +352,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1">
-        <v>864.11400000000003</v>
+        <v>940.52800000000002</v>
       </c>
       <c r="B1" s="1">
-        <v>1019.347</v>
+        <v>1019.168</v>
       </c>
       <c r="C1" s="1">
-        <v>2501.1</v>
+        <v>2501.1999999999998</v>
       </c>
       <c r="D1" s="1">
         <v>0</v>
@@ -367,193 +367,193 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>885.55</v>
+        <v>974.19399999999996</v>
       </c>
       <c r="B2" s="1">
-        <v>1778.527</v>
+        <v>1793.377</v>
       </c>
       <c r="C2" s="1">
-        <v>2501.1</v>
+        <v>2501.1999999999998</v>
       </c>
       <c r="D2" s="1">
-        <v>-16.07</v>
+        <v>-15.93</v>
       </c>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <v>880.46</v>
+        <v>967.72199999999998</v>
       </c>
       <c r="B3" s="1">
-        <v>1673.99</v>
+        <v>1697.279</v>
       </c>
       <c r="C3" s="1">
-        <v>2501.1</v>
+        <v>2501.1999999999998</v>
       </c>
       <c r="D3" s="1">
-        <v>-13.95</v>
+        <v>-14.02</v>
       </c>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>876.44899999999996</v>
+        <v>961.42200000000003</v>
       </c>
       <c r="B4" s="1">
-        <v>1576.57</v>
+        <v>1597.1289999999999</v>
       </c>
       <c r="C4" s="1">
-        <v>2501.1</v>
+        <v>2501.1999999999998</v>
       </c>
       <c r="D4" s="1">
-        <v>-11.93</v>
+        <v>-12</v>
       </c>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
-        <v>872.82299999999998</v>
+        <v>956.20899999999995</v>
       </c>
       <c r="B5" s="1">
-        <v>1481.614</v>
+        <v>1499.7429999999999</v>
       </c>
       <c r="C5" s="1">
-        <v>2501.1</v>
+        <v>2501.1999999999998</v>
       </c>
       <c r="D5" s="1">
-        <v>-9.93</v>
+        <v>-10</v>
       </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
-        <v>870.03399999999999</v>
+        <v>951.48400000000004</v>
       </c>
       <c r="B6" s="1">
-        <v>1387.847</v>
+        <v>1401.5150000000001</v>
       </c>
       <c r="C6" s="1">
-        <v>2501.1</v>
+        <v>2501.1999999999998</v>
       </c>
       <c r="D6" s="1">
-        <v>-7.95</v>
+        <v>-8.1</v>
       </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
-        <v>867.721</v>
+        <v>947.452</v>
       </c>
       <c r="B7" s="1">
-        <v>1292.8630000000001</v>
+        <v>1301.2070000000001</v>
       </c>
       <c r="C7" s="1">
-        <v>2501.1</v>
+        <v>2501.1999999999998</v>
       </c>
       <c r="D7" s="1">
-        <v>-5.93</v>
+        <v>-6</v>
       </c>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
-        <v>865.90899999999999</v>
+        <v>944.45699999999999</v>
       </c>
       <c r="B8" s="1">
-        <v>1200.325</v>
+        <v>1206.1579999999999</v>
       </c>
       <c r="C8" s="1">
-        <v>2501.1</v>
+        <v>2501.1999999999998</v>
       </c>
       <c r="D8" s="1">
-        <v>-3.93</v>
+        <v>-3.97</v>
       </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
-        <v>864.89400000000001</v>
+        <v>942.28700000000003</v>
       </c>
       <c r="B9" s="1">
-        <v>1108.3440000000001</v>
+        <v>1112.0640000000001</v>
       </c>
       <c r="C9" s="1">
-        <v>2501.1</v>
+        <v>2501.1999999999998</v>
       </c>
       <c r="D9" s="1">
-        <v>-1.95</v>
+        <v>-2</v>
       </c>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
-        <v>864.08500000000004</v>
+        <v>940.51099999999997</v>
       </c>
       <c r="B10" s="1">
-        <v>1014.44</v>
+        <v>1016.948</v>
       </c>
       <c r="C10" s="1">
-        <v>2501.1</v>
+        <v>2501.1999999999998</v>
       </c>
       <c r="D10" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>0.03</v>
       </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
-        <v>864.24599999999998</v>
+        <v>939.65800000000002</v>
       </c>
       <c r="B11" s="1">
-        <v>922.71</v>
+        <v>924.05899999999997</v>
       </c>
       <c r="C11" s="1">
-        <v>2501.1</v>
+        <v>2501.1999999999998</v>
       </c>
       <c r="D11" s="1">
-        <v>2.02</v>
+        <v>2.0299999999999998</v>
       </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
-        <v>864.93700000000001</v>
+        <v>939.59199999999998</v>
       </c>
       <c r="B12" s="1">
-        <v>828.10500000000002</v>
+        <v>830.86</v>
       </c>
       <c r="C12" s="1">
-        <v>2501.1</v>
+        <v>2501.1999999999998</v>
       </c>
       <c r="D12" s="1">
-        <v>4.07</v>
+        <v>4.03</v>
       </c>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
-        <v>866.14800000000002</v>
+        <v>940.21299999999997</v>
       </c>
       <c r="B13" s="1">
-        <v>735.21400000000006</v>
+        <v>736.54700000000003</v>
       </c>
       <c r="C13" s="1">
-        <v>2501.1</v>
+        <v>2501.1999999999998</v>
       </c>
       <c r="D13" s="1">
-        <v>6.05</v>
+        <v>6</v>
       </c>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
-        <v>867.91700000000003</v>
+        <v>941.851</v>
       </c>
       <c r="B14" s="1">
-        <v>641.06100000000004</v>
+        <v>640.47199999999998</v>
       </c>
       <c r="C14" s="1">
-        <v>2501.1</v>
+        <v>2501.1999999999998</v>
       </c>
       <c r="D14" s="1">
         <v>8.0500000000000007</v>
@@ -562,73 +562,73 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
-        <v>870.45299999999997</v>
+        <v>943.67600000000004</v>
       </c>
       <c r="B15" s="1">
-        <v>546.29200000000003</v>
+        <v>546.49800000000005</v>
       </c>
       <c r="C15" s="1">
-        <v>2501.1</v>
+        <v>2501.1999999999998</v>
       </c>
       <c r="D15" s="1">
-        <v>10.02</v>
+        <v>10.029999999999999</v>
       </c>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
-        <v>873.50900000000001</v>
+        <v>946.59100000000001</v>
       </c>
       <c r="B16" s="1">
-        <v>447.89699999999999</v>
+        <v>449.82400000000001</v>
       </c>
       <c r="C16" s="1">
-        <v>2501.1</v>
+        <v>2501.1999999999998</v>
       </c>
       <c r="D16" s="1">
-        <v>12.02</v>
+        <v>12.03</v>
       </c>
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
-        <v>877.13699999999994</v>
+        <v>950.077</v>
       </c>
       <c r="B17" s="1">
-        <v>349.91899999999998</v>
+        <v>351.76299999999998</v>
       </c>
       <c r="C17" s="1">
-        <v>2501.1</v>
+        <v>2501.1999999999998</v>
       </c>
       <c r="D17" s="1">
-        <v>14.07</v>
+        <v>14.03</v>
       </c>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
-        <v>881.27</v>
+        <v>954.23299999999995</v>
       </c>
       <c r="B18" s="1">
-        <v>251.999</v>
+        <v>252.71100000000001</v>
       </c>
       <c r="C18" s="1">
-        <v>2501.1</v>
+        <v>2501.1999999999998</v>
       </c>
       <c r="D18" s="1">
-        <v>16.05</v>
+        <v>16.02</v>
       </c>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
-        <v>845.04200000000003</v>
+        <v>921.74400000000003</v>
       </c>
       <c r="B19" s="1">
-        <v>1019.205</v>
+        <v>1019.15</v>
       </c>
       <c r="C19" s="1">
-        <v>2600.8000000000002</v>
+        <v>2600.9</v>
       </c>
       <c r="D19" s="1">
         <v>0</v>
@@ -637,268 +637,268 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
-        <v>865.93399999999997</v>
+        <v>954.76099999999997</v>
       </c>
       <c r="B20" s="1">
-        <v>1777.903</v>
+        <v>1792.7629999999999</v>
       </c>
       <c r="C20" s="1">
-        <v>2600.8000000000002</v>
+        <v>2600.9</v>
       </c>
       <c r="D20" s="1">
-        <v>-16.100000000000001</v>
+        <v>-15.92</v>
       </c>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
-        <v>860.99300000000005</v>
+        <v>948.12699999999995</v>
       </c>
       <c r="B21" s="1">
-        <v>1671.4590000000001</v>
+        <v>1695.704</v>
       </c>
       <c r="C21" s="1">
-        <v>2600.8000000000002</v>
+        <v>2600.9</v>
       </c>
       <c r="D21" s="1">
-        <v>-13.95</v>
+        <v>-14.05</v>
       </c>
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
-        <v>857.02599999999995</v>
+        <v>942.23</v>
       </c>
       <c r="B22" s="1">
-        <v>1574.2940000000001</v>
+        <v>1595.482</v>
       </c>
       <c r="C22" s="1">
-        <v>2600.8000000000002</v>
+        <v>2600.9</v>
       </c>
       <c r="D22" s="1">
-        <v>-11.92</v>
+        <v>-12</v>
       </c>
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
-        <v>853.596</v>
+        <v>937.00400000000002</v>
       </c>
       <c r="B23" s="1">
-        <v>1479.7149999999999</v>
+        <v>1497.596</v>
       </c>
       <c r="C23" s="1">
-        <v>2600.8000000000002</v>
+        <v>2600.9</v>
       </c>
       <c r="D23" s="1">
-        <v>-9.92</v>
+        <v>-9.9700000000000006</v>
       </c>
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
-        <v>850.75199999999995</v>
+        <v>932.47</v>
       </c>
       <c r="B24" s="1">
-        <v>1385.6479999999999</v>
+        <v>1402.145</v>
       </c>
       <c r="C24" s="1">
-        <v>2600.8000000000002</v>
+        <v>2600.9</v>
       </c>
       <c r="D24" s="1">
-        <v>-7.95</v>
+        <v>-8.1</v>
       </c>
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
-        <v>848.46</v>
+        <v>928.51300000000003</v>
       </c>
       <c r="B25" s="1">
-        <v>1291.2560000000001</v>
+        <v>1302.3710000000001</v>
       </c>
       <c r="C25" s="1">
-        <v>2600.8000000000002</v>
+        <v>2600.9</v>
       </c>
       <c r="D25" s="1">
-        <v>-5.92</v>
+        <v>-6</v>
       </c>
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
-        <v>846.75900000000001</v>
+        <v>925.53200000000004</v>
       </c>
       <c r="B26" s="1">
-        <v>1198.9829999999999</v>
+        <v>1206.7349999999999</v>
       </c>
       <c r="C26" s="1">
-        <v>2600.8000000000002</v>
+        <v>2600.9</v>
       </c>
       <c r="D26" s="1">
-        <v>-3.92</v>
+        <v>-4</v>
       </c>
       <c r="E26" s="1"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
-        <v>845.63599999999997</v>
+        <v>923.25400000000002</v>
       </c>
       <c r="B27" s="1">
-        <v>1107.241</v>
+        <v>1111.289</v>
       </c>
       <c r="C27" s="1">
-        <v>2600.8000000000002</v>
+        <v>2600.9</v>
       </c>
       <c r="D27" s="1">
-        <v>-1.95</v>
+        <v>-2</v>
       </c>
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
-        <v>845.13900000000001</v>
+        <v>921.66</v>
       </c>
       <c r="B28" s="1">
-        <v>1013.897</v>
+        <v>1017.107</v>
       </c>
       <c r="C28" s="1">
-        <v>2600.8000000000002</v>
+        <v>2600.9</v>
       </c>
       <c r="D28" s="1">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
       <c r="E28" s="1"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
-        <v>845.23900000000003</v>
+        <v>920.87699999999995</v>
       </c>
       <c r="B29" s="1">
-        <v>922.20399999999995</v>
+        <v>924.04600000000005</v>
       </c>
       <c r="C29" s="1">
-        <v>2600.8000000000002</v>
+        <v>2600.9</v>
       </c>
       <c r="D29" s="1">
-        <v>2.02</v>
+        <v>2.0299999999999998</v>
       </c>
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
-        <v>845.73599999999999</v>
+        <v>920.64099999999996</v>
       </c>
       <c r="B30" s="1">
-        <v>827.303</v>
+        <v>830.97299999999996</v>
       </c>
       <c r="C30" s="1">
-        <v>2600.8000000000002</v>
+        <v>2600.9</v>
       </c>
       <c r="D30" s="1">
-        <v>4.08</v>
+        <v>4.03</v>
       </c>
       <c r="E30" s="1"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
-        <v>846.976</v>
+        <v>921.43899999999996</v>
       </c>
       <c r="B31" s="1">
-        <v>734.89300000000003</v>
+        <v>736.85799999999995</v>
       </c>
       <c r="C31" s="1">
-        <v>2600.8000000000002</v>
+        <v>2600.9</v>
       </c>
       <c r="D31" s="1">
-        <v>6.05</v>
+        <v>6.03</v>
       </c>
       <c r="E31" s="1"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
-        <v>848.80100000000004</v>
+        <v>922.85500000000002</v>
       </c>
       <c r="B32" s="1">
-        <v>640.01700000000005</v>
+        <v>642.21</v>
       </c>
       <c r="C32" s="1">
-        <v>2600.8000000000002</v>
+        <v>2600.9</v>
       </c>
       <c r="D32" s="1">
-        <v>8.0500000000000007</v>
+        <v>8.0299999999999994</v>
       </c>
       <c r="E32" s="1"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
-        <v>851.23699999999997</v>
+        <v>924.68299999999999</v>
       </c>
       <c r="B33" s="1">
-        <v>546.02200000000005</v>
+        <v>546.38599999999997</v>
       </c>
       <c r="C33" s="1">
-        <v>2600.8000000000002</v>
+        <v>2600.9</v>
       </c>
       <c r="D33" s="1">
-        <v>10.02</v>
+        <v>10.050000000000001</v>
       </c>
       <c r="E33" s="1"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
-        <v>854.279</v>
+        <v>927.43700000000001</v>
       </c>
       <c r="B34" s="1">
-        <v>448.41699999999997</v>
+        <v>451.21199999999999</v>
       </c>
       <c r="C34" s="1">
-        <v>2600.8000000000002</v>
+        <v>2600.9</v>
       </c>
       <c r="D34" s="1">
-        <v>12.02</v>
+        <v>12.03</v>
       </c>
       <c r="E34" s="1"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
-        <v>857.66899999999998</v>
+        <v>930.73299999999995</v>
       </c>
       <c r="B35" s="1">
-        <v>350.19299999999998</v>
+        <v>354.00400000000002</v>
       </c>
       <c r="C35" s="1">
-        <v>2600.8000000000002</v>
+        <v>2600.9</v>
       </c>
       <c r="D35" s="1">
-        <v>14.08</v>
+        <v>14.03</v>
       </c>
       <c r="E35" s="1"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
-        <v>861.77800000000002</v>
+        <v>934.56200000000001</v>
       </c>
       <c r="B36" s="1">
-        <v>252.102</v>
+        <v>255.38300000000001</v>
       </c>
       <c r="C36" s="1">
-        <v>2600.8000000000002</v>
+        <v>2600.9</v>
       </c>
       <c r="D36" s="1">
-        <v>16.05</v>
+        <v>16.03</v>
       </c>
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
-        <v>827.67100000000005</v>
+        <v>904.43299999999999</v>
       </c>
       <c r="B37" s="1">
-        <v>1019.1609999999999</v>
+        <v>1019.401</v>
       </c>
       <c r="C37" s="1">
-        <v>2700.5</v>
+        <v>2700.6</v>
       </c>
       <c r="D37" s="1">
         <v>0</v>
@@ -907,238 +907,238 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
-        <v>847.93399999999997</v>
+        <v>936.63099999999997</v>
       </c>
       <c r="B38" s="1">
-        <v>1777.675</v>
+        <v>1792.771</v>
       </c>
       <c r="C38" s="1">
-        <v>2700.5</v>
+        <v>2700.6</v>
       </c>
       <c r="D38" s="1">
-        <v>-16.100000000000001</v>
+        <v>-15.95</v>
       </c>
       <c r="E38" s="1"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
-        <v>842.95</v>
+        <v>930.48500000000001</v>
       </c>
       <c r="B39" s="1">
-        <v>1671.1220000000001</v>
+        <v>1695.617</v>
       </c>
       <c r="C39" s="1">
-        <v>2700.5</v>
+        <v>2700.6</v>
       </c>
       <c r="D39" s="1">
-        <v>-13.95</v>
+        <v>-14.05</v>
       </c>
       <c r="E39" s="1"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
-        <v>839.18799999999999</v>
+        <v>924.43299999999999</v>
       </c>
       <c r="B40" s="1">
-        <v>1573.675</v>
+        <v>1594.096</v>
       </c>
       <c r="C40" s="1">
-        <v>2700.5</v>
+        <v>2700.6</v>
       </c>
       <c r="D40" s="1">
-        <v>-11.92</v>
+        <v>-12</v>
       </c>
       <c r="E40" s="1"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
-        <v>835.76300000000003</v>
+        <v>919.33299999999997</v>
       </c>
       <c r="B41" s="1">
-        <v>1480.2339999999999</v>
+        <v>1496.7840000000001</v>
       </c>
       <c r="C41" s="1">
-        <v>2700.5</v>
+        <v>2700.6</v>
       </c>
       <c r="D41" s="1">
-        <v>-9.92</v>
+        <v>-9.9700000000000006</v>
       </c>
       <c r="E41" s="1"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
-        <v>833.29399999999998</v>
+        <v>915.077</v>
       </c>
       <c r="B42" s="1">
-        <v>1387.415</v>
+        <v>1401.502</v>
       </c>
       <c r="C42" s="1">
-        <v>2700.5</v>
+        <v>2700.6</v>
       </c>
       <c r="D42" s="1">
-        <v>-7.98</v>
+        <v>-8.1</v>
       </c>
       <c r="E42" s="1"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
-        <v>830.99400000000003</v>
+        <v>911.01300000000003</v>
       </c>
       <c r="B43" s="1">
-        <v>1292.306</v>
+        <v>1301.3430000000001</v>
       </c>
       <c r="C43" s="1">
-        <v>2700.5</v>
+        <v>2700.6</v>
       </c>
       <c r="D43" s="1">
-        <v>-5.92</v>
+        <v>-6</v>
       </c>
       <c r="E43" s="1"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
-        <v>829.12199999999996</v>
+        <v>908.22299999999996</v>
       </c>
       <c r="B44" s="1">
-        <v>1199.912</v>
+        <v>1206.2529999999999</v>
       </c>
       <c r="C44" s="1">
-        <v>2700.5</v>
+        <v>2700.6</v>
       </c>
       <c r="D44" s="1">
-        <v>-3.92</v>
+        <v>-4</v>
       </c>
       <c r="E44" s="1"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
-        <v>828.15300000000002</v>
+        <v>905.84799999999996</v>
       </c>
       <c r="B45" s="1">
-        <v>1107.923</v>
+        <v>1111.221</v>
       </c>
       <c r="C45" s="1">
-        <v>2700.5</v>
+        <v>2700.6</v>
       </c>
       <c r="D45" s="1">
-        <v>-1.95</v>
+        <v>-2</v>
       </c>
       <c r="E45" s="1"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
-        <v>827.62099999999998</v>
+        <v>904.39200000000005</v>
       </c>
       <c r="B46" s="1">
-        <v>1014.54</v>
+        <v>1016.737</v>
       </c>
       <c r="C46" s="1">
-        <v>2700.5</v>
+        <v>2700.6</v>
       </c>
       <c r="D46" s="1">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="E46" s="1"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
-        <v>827.85799999999995</v>
+        <v>903.42200000000003</v>
       </c>
       <c r="B47" s="1">
-        <v>922.15200000000004</v>
+        <v>923.51800000000003</v>
       </c>
       <c r="C47" s="1">
-        <v>2700.5</v>
+        <v>2700.6</v>
       </c>
       <c r="D47" s="1">
-        <v>2.0499999999999998</v>
+        <v>2.0299999999999998</v>
       </c>
       <c r="E47" s="1"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
-        <v>828.18600000000004</v>
+        <v>903.43499999999995</v>
       </c>
       <c r="B48" s="1">
-        <v>828.55799999999999</v>
+        <v>830.33399999999995</v>
       </c>
       <c r="C48" s="1">
-        <v>2700.5</v>
+        <v>2700.6</v>
       </c>
       <c r="D48" s="1">
-        <v>4.05</v>
+        <v>4.03</v>
       </c>
       <c r="E48" s="1"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
-        <v>829.65700000000004</v>
+        <v>903.846</v>
       </c>
       <c r="B49" s="1">
-        <v>734.44200000000001</v>
+        <v>736.50599999999997</v>
       </c>
       <c r="C49" s="1">
-        <v>2700.5</v>
+        <v>2700.6</v>
       </c>
       <c r="D49" s="1">
-        <v>6.05</v>
+        <v>6.03</v>
       </c>
       <c r="E49" s="1"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
-        <v>831.12900000000002</v>
+        <v>905.08500000000004</v>
       </c>
       <c r="B50" s="1">
-        <v>640.47699999999998</v>
+        <v>642.03499999999997</v>
       </c>
       <c r="C50" s="1">
-        <v>2700.5</v>
+        <v>2700.6</v>
       </c>
       <c r="D50" s="1">
-        <v>8.0500000000000007</v>
+        <v>8.0299999999999994</v>
       </c>
       <c r="E50" s="1"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
-        <v>833.36800000000005</v>
+        <v>906.95500000000004</v>
       </c>
       <c r="B51" s="1">
-        <v>546.15200000000004</v>
+        <v>547.07600000000002</v>
       </c>
       <c r="C51" s="1">
-        <v>2700.5</v>
+        <v>2700.6</v>
       </c>
       <c r="D51" s="1">
-        <v>10.02</v>
+        <v>10.029999999999999</v>
       </c>
       <c r="E51" s="1"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
-        <v>836.452</v>
+        <v>909.62099999999998</v>
       </c>
       <c r="B52" s="1">
-        <v>448.49099999999999</v>
+        <v>450.85199999999998</v>
       </c>
       <c r="C52" s="1">
-        <v>2700.5</v>
+        <v>2700.6</v>
       </c>
       <c r="D52" s="1">
-        <v>12.05</v>
+        <v>12.03</v>
       </c>
       <c r="E52" s="1"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
-        <v>839.54200000000003</v>
+        <v>912.94600000000003</v>
       </c>
       <c r="B53" s="1">
-        <v>351.87599999999998</v>
+        <v>352.90800000000002</v>
       </c>
       <c r="C53" s="1">
-        <v>2700.5</v>
+        <v>2700.6</v>
       </c>
       <c r="D53" s="1">
         <v>14.05</v>
@@ -1147,28 +1147,28 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
-        <v>843.553</v>
+        <v>916.55</v>
       </c>
       <c r="B54" s="1">
-        <v>253.03399999999999</v>
+        <v>255.81200000000001</v>
       </c>
       <c r="C54" s="1">
-        <v>2700.5</v>
+        <v>2700.6</v>
       </c>
       <c r="D54" s="1">
-        <v>16.079999999999998</v>
+        <v>16.03</v>
       </c>
       <c r="E54" s="1"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
-        <v>811.48699999999997</v>
+        <v>888.32</v>
       </c>
       <c r="B55" s="1">
-        <v>1019.562</v>
+        <v>1019.26</v>
       </c>
       <c r="C55" s="1">
-        <v>2800.2</v>
+        <v>2800.3</v>
       </c>
       <c r="D55" s="1">
         <v>0</v>
@@ -1177,163 +1177,163 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
-        <v>830.90599999999995</v>
+        <v>919.83799999999997</v>
       </c>
       <c r="B56" s="1">
-        <v>1776.954</v>
+        <v>1791.778</v>
       </c>
       <c r="C56" s="1">
-        <v>2800.2</v>
+        <v>2800.3</v>
       </c>
       <c r="D56" s="1">
-        <v>-16.100000000000001</v>
+        <v>-15.93</v>
       </c>
       <c r="E56" s="1"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
-        <v>826.17600000000004</v>
+        <v>913.77800000000002</v>
       </c>
       <c r="B57" s="1">
-        <v>1670.383</v>
+        <v>1695.8130000000001</v>
       </c>
       <c r="C57" s="1">
-        <v>2800.2</v>
+        <v>2800.3</v>
       </c>
       <c r="D57" s="1">
-        <v>-13.95</v>
+        <v>-14.05</v>
       </c>
       <c r="E57" s="1"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
-        <v>822.53200000000004</v>
+        <v>908.02499999999998</v>
       </c>
       <c r="B58" s="1">
-        <v>1573.7670000000001</v>
+        <v>1594.627</v>
       </c>
       <c r="C58" s="1">
-        <v>2800.2</v>
+        <v>2800.3</v>
       </c>
       <c r="D58" s="1">
-        <v>-11.92</v>
+        <v>-12</v>
       </c>
       <c r="E58" s="1"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
-        <v>819.46299999999997</v>
+        <v>902.79</v>
       </c>
       <c r="B59" s="1">
-        <v>1479.316</v>
+        <v>1497.58</v>
       </c>
       <c r="C59" s="1">
-        <v>2800.2</v>
+        <v>2800.3</v>
       </c>
       <c r="D59" s="1">
-        <v>-9.92</v>
+        <v>-10</v>
       </c>
       <c r="E59" s="1"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
-        <v>816.89800000000002</v>
+        <v>898.53700000000003</v>
       </c>
       <c r="B60" s="1">
-        <v>1387.4760000000001</v>
+        <v>1400.2639999999999</v>
       </c>
       <c r="C60" s="1">
-        <v>2800.2</v>
+        <v>2800.3</v>
       </c>
       <c r="D60" s="1">
-        <v>-7.98</v>
+        <v>-8.08</v>
       </c>
       <c r="E60" s="1"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
-        <v>814.69600000000003</v>
+        <v>894.88800000000003</v>
       </c>
       <c r="B61" s="1">
-        <v>1292.0039999999999</v>
+        <v>1302.0530000000001</v>
       </c>
       <c r="C61" s="1">
-        <v>2800.2</v>
+        <v>2800.3</v>
       </c>
       <c r="D61" s="1">
-        <v>-5.92</v>
+        <v>-6</v>
       </c>
       <c r="E61" s="1"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
-        <v>813.00300000000004</v>
+        <v>891.98900000000003</v>
       </c>
       <c r="B62" s="1">
-        <v>1199.732</v>
+        <v>1206.4580000000001</v>
       </c>
       <c r="C62" s="1">
-        <v>2800.2</v>
+        <v>2800.3</v>
       </c>
       <c r="D62" s="1">
-        <v>-3.92</v>
+        <v>-3.98</v>
       </c>
       <c r="E62" s="1"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
-        <v>811.93100000000004</v>
+        <v>889.83199999999999</v>
       </c>
       <c r="B63" s="1">
-        <v>1108.502</v>
+        <v>1113.1990000000001</v>
       </c>
       <c r="C63" s="1">
-        <v>2800.2</v>
+        <v>2800.3</v>
       </c>
       <c r="D63" s="1">
-        <v>-1.95</v>
+        <v>-2</v>
       </c>
       <c r="E63" s="1"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
-        <v>811.43499999999995</v>
+        <v>888.29</v>
       </c>
       <c r="B64" s="1">
-        <v>1014.937</v>
+        <v>1018.417</v>
       </c>
       <c r="C64" s="1">
-        <v>2800.2</v>
+        <v>2800.3</v>
       </c>
       <c r="D64" s="1">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="E64" s="1"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
-        <v>811.226</v>
+        <v>887.40300000000002</v>
       </c>
       <c r="B65" s="1">
-        <v>921.89800000000002</v>
+        <v>925.41800000000001</v>
       </c>
       <c r="C65" s="1">
-        <v>2800.2</v>
+        <v>2800.3</v>
       </c>
       <c r="D65" s="1">
-        <v>2.0499999999999998</v>
+        <v>2</v>
       </c>
       <c r="E65" s="1"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
-        <v>811.84400000000005</v>
+        <v>887.17899999999997</v>
       </c>
       <c r="B66" s="1">
-        <v>829.31899999999996</v>
+        <v>830.80399999999997</v>
       </c>
       <c r="C66" s="1">
-        <v>2800.2</v>
+        <v>2800.3</v>
       </c>
       <c r="D66" s="1">
         <v>4.05</v>
@@ -1342,28 +1342,28 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
-        <v>813.05200000000002</v>
+        <v>887.57500000000005</v>
       </c>
       <c r="B67" s="1">
-        <v>735.40300000000002</v>
+        <v>738.06</v>
       </c>
       <c r="C67" s="1">
-        <v>2800.2</v>
+        <v>2800.3</v>
       </c>
       <c r="D67" s="1">
-        <v>6.05</v>
+        <v>6</v>
       </c>
       <c r="E67" s="1"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
-        <v>814.86400000000003</v>
+        <v>888.85699999999997</v>
       </c>
       <c r="B68" s="1">
-        <v>641.97900000000004</v>
+        <v>642.47</v>
       </c>
       <c r="C68" s="1">
-        <v>2800.2</v>
+        <v>2800.3</v>
       </c>
       <c r="D68" s="1">
         <v>8.0500000000000007</v>
@@ -1372,73 +1372,73 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
-        <v>816.76800000000003</v>
+        <v>890.70799999999997</v>
       </c>
       <c r="B69" s="1">
-        <v>546.04600000000005</v>
+        <v>548.21900000000005</v>
       </c>
       <c r="C69" s="1">
-        <v>2800.2</v>
+        <v>2800.3</v>
       </c>
       <c r="D69" s="1">
-        <v>10.050000000000001</v>
+        <v>10.02</v>
       </c>
       <c r="E69" s="1"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
-        <v>819.53300000000002</v>
+        <v>893.096</v>
       </c>
       <c r="B70" s="1">
-        <v>450.40600000000001</v>
+        <v>452.70800000000003</v>
       </c>
       <c r="C70" s="1">
-        <v>2800.2</v>
+        <v>2800.3</v>
       </c>
       <c r="D70" s="1">
-        <v>12.02</v>
+        <v>12.05</v>
       </c>
       <c r="E70" s="1"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
-        <v>822.92499999999995</v>
+        <v>896.03599999999994</v>
       </c>
       <c r="B71" s="1">
-        <v>352.27300000000002</v>
+        <v>357.24799999999999</v>
       </c>
       <c r="C71" s="1">
-        <v>2800.2</v>
+        <v>2800.3</v>
       </c>
       <c r="D71" s="1">
-        <v>14.05</v>
+        <v>14.02</v>
       </c>
       <c r="E71" s="1"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
-        <v>826.61699999999996</v>
+        <v>899.71100000000001</v>
       </c>
       <c r="B72" s="1">
-        <v>254.46700000000001</v>
+        <v>257.05200000000002</v>
       </c>
       <c r="C72" s="1">
-        <v>2800.2</v>
+        <v>2800.3</v>
       </c>
       <c r="D72" s="1">
-        <v>16.079999999999998</v>
+        <v>16.02</v>
       </c>
       <c r="E72" s="1"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
-        <v>796.173</v>
+        <v>873.18700000000001</v>
       </c>
       <c r="B73" s="1">
-        <v>1019.22</v>
+        <v>1019.168</v>
       </c>
       <c r="C73" s="1">
-        <v>2899.9</v>
+        <v>2900</v>
       </c>
       <c r="D73" s="1">
         <v>0</v>
@@ -1447,163 +1447,163 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
-        <v>815.20299999999997</v>
+        <v>904.26800000000003</v>
       </c>
       <c r="B74" s="1">
-        <v>1775.8309999999999</v>
+        <v>1790.653</v>
       </c>
       <c r="C74" s="1">
-        <v>2899.9</v>
+        <v>2900</v>
       </c>
       <c r="D74" s="1">
-        <v>-16.100000000000001</v>
+        <v>-15.95</v>
       </c>
       <c r="E74" s="1"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
-        <v>810.73400000000004</v>
+        <v>898.36300000000006</v>
       </c>
       <c r="B75" s="1">
-        <v>1669.3309999999999</v>
+        <v>1693.76</v>
       </c>
       <c r="C75" s="1">
-        <v>2899.9</v>
+        <v>2900</v>
       </c>
       <c r="D75" s="1">
-        <v>-13.95</v>
+        <v>-14.03</v>
       </c>
       <c r="E75" s="1"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
-        <v>807.10500000000002</v>
+        <v>892.67600000000004</v>
       </c>
       <c r="B76" s="1">
-        <v>1574.191</v>
+        <v>1594.537</v>
       </c>
       <c r="C76" s="1">
-        <v>2899.9</v>
+        <v>2900</v>
       </c>
       <c r="D76" s="1">
-        <v>-11.92</v>
+        <v>-12</v>
       </c>
       <c r="E76" s="1"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
-        <v>804.20399999999995</v>
+        <v>887.57299999999998</v>
       </c>
       <c r="B77" s="1">
-        <v>1480.9839999999999</v>
+        <v>1496.7760000000001</v>
       </c>
       <c r="C77" s="1">
-        <v>2899.9</v>
+        <v>2900</v>
       </c>
       <c r="D77" s="1">
-        <v>-9.9499999999999993</v>
+        <v>-10</v>
       </c>
       <c r="E77" s="1"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
-        <v>801.52499999999998</v>
+        <v>883.45799999999997</v>
       </c>
       <c r="B78" s="1">
-        <v>1385.8389999999999</v>
+        <v>1400.202</v>
       </c>
       <c r="C78" s="1">
-        <v>2899.9</v>
+        <v>2900</v>
       </c>
       <c r="D78" s="1">
-        <v>-7.95</v>
+        <v>-8.08</v>
       </c>
       <c r="E78" s="1"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
-        <v>799.33299999999997</v>
+        <v>879.74400000000003</v>
       </c>
       <c r="B79" s="1">
-        <v>1291.934</v>
+        <v>1300.7809999999999</v>
       </c>
       <c r="C79" s="1">
-        <v>2899.9</v>
+        <v>2900</v>
       </c>
       <c r="D79" s="1">
-        <v>-5.92</v>
+        <v>-6</v>
       </c>
       <c r="E79" s="1"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
-        <v>797.85400000000004</v>
+        <v>876.99</v>
       </c>
       <c r="B80" s="1">
-        <v>1200.001</v>
+        <v>1206.018</v>
       </c>
       <c r="C80" s="1">
-        <v>2899.9</v>
+        <v>2900</v>
       </c>
       <c r="D80" s="1">
-        <v>-3.92</v>
+        <v>-3.98</v>
       </c>
       <c r="E80" s="1"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
-        <v>796.74699999999996</v>
+        <v>874.75300000000004</v>
       </c>
       <c r="B81" s="1">
-        <v>1108.3599999999999</v>
+        <v>1112.3969999999999</v>
       </c>
       <c r="C81" s="1">
-        <v>2899.9</v>
+        <v>2900</v>
       </c>
       <c r="D81" s="1">
-        <v>-1.95</v>
+        <v>-2</v>
       </c>
       <c r="E81" s="1"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
-        <v>796.18299999999999</v>
+        <v>873.15</v>
       </c>
       <c r="B82" s="1">
-        <v>1015.529</v>
+        <v>1017.968</v>
       </c>
       <c r="C82" s="1">
-        <v>2899.9</v>
+        <v>2900</v>
       </c>
       <c r="D82" s="1">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="E82" s="1"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
-        <v>796.26599999999996</v>
+        <v>872.42200000000003</v>
       </c>
       <c r="B83" s="1">
-        <v>921.553</v>
+        <v>924.92100000000005</v>
       </c>
       <c r="C83" s="1">
-        <v>2899.9</v>
+        <v>2900</v>
       </c>
       <c r="D83" s="1">
-        <v>2.0499999999999998</v>
+        <v>2</v>
       </c>
       <c r="E83" s="1"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
-        <v>796.83</v>
+        <v>872.20600000000002</v>
       </c>
       <c r="B84" s="1">
-        <v>829.36</v>
+        <v>830.75</v>
       </c>
       <c r="C84" s="1">
-        <v>2899.9</v>
+        <v>2900</v>
       </c>
       <c r="D84" s="1">
         <v>4.05</v>
@@ -1612,58 +1612,58 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
-        <v>797.83299999999997</v>
+        <v>872.60400000000004</v>
       </c>
       <c r="B85" s="1">
-        <v>735.85199999999998</v>
+        <v>738.303</v>
       </c>
       <c r="C85" s="1">
-        <v>2899.9</v>
+        <v>2900</v>
       </c>
       <c r="D85" s="1">
-        <v>6.08</v>
+        <v>6</v>
       </c>
       <c r="E85" s="1"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
-        <v>799.66</v>
+        <v>873.77700000000004</v>
       </c>
       <c r="B86" s="1">
-        <v>643.42700000000002</v>
+        <v>642.77800000000002</v>
       </c>
       <c r="C86" s="1">
-        <v>2899.9</v>
+        <v>2900</v>
       </c>
       <c r="D86" s="1">
-        <v>8.02</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="E86" s="1"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
-        <v>801.73699999999997</v>
+        <v>875.43100000000004</v>
       </c>
       <c r="B87" s="1">
-        <v>547.46199999999999</v>
+        <v>548.88699999999994</v>
       </c>
       <c r="C87" s="1">
-        <v>2899.9</v>
+        <v>2900</v>
       </c>
       <c r="D87" s="1">
-        <v>10.050000000000001</v>
+        <v>10.02</v>
       </c>
       <c r="E87" s="1"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
-        <v>804.14800000000002</v>
+        <v>877.86900000000003</v>
       </c>
       <c r="B88" s="1">
-        <v>451.76400000000001</v>
+        <v>453.06400000000002</v>
       </c>
       <c r="C88" s="1">
-        <v>2899.9</v>
+        <v>2900</v>
       </c>
       <c r="D88" s="1">
         <v>12.02</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
-        <v>807.21400000000006</v>
+        <v>880.88800000000003</v>
       </c>
       <c r="B89" s="1">
-        <v>353.18599999999998</v>
+        <v>355.887</v>
       </c>
       <c r="C89" s="1">
-        <v>2899.9</v>
+        <v>2900</v>
       </c>
       <c r="D89" s="1">
         <v>14.05</v>
@@ -1687,28 +1687,28 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
-        <v>810.85299999999995</v>
+        <v>884.30799999999999</v>
       </c>
       <c r="B90" s="1">
-        <v>255.239</v>
+        <v>257.714</v>
       </c>
       <c r="C90" s="1">
-        <v>2899.9</v>
+        <v>2900</v>
       </c>
       <c r="D90" s="1">
-        <v>16.079999999999998</v>
+        <v>16.02</v>
       </c>
       <c r="E90" s="1"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
-        <v>782.29300000000001</v>
+        <v>859.31299999999999</v>
       </c>
       <c r="B91" s="1">
-        <v>1019.313</v>
+        <v>1019.399</v>
       </c>
       <c r="C91" s="1">
-        <v>2999.5</v>
+        <v>2999.6</v>
       </c>
       <c r="D91" s="1">
         <v>0</v>
@@ -1717,256 +1717,256 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
-        <v>800.62900000000002</v>
+        <v>889.76400000000001</v>
       </c>
       <c r="B92" s="1">
-        <v>1775.425</v>
+        <v>1789.8979999999999</v>
       </c>
       <c r="C92" s="1">
-        <v>2999.5</v>
+        <v>2999.6</v>
       </c>
       <c r="D92" s="1">
-        <v>-16.100000000000001</v>
+        <v>-15.95</v>
       </c>
       <c r="E92" s="1"/>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
-        <v>796.12900000000002</v>
+        <v>883.90200000000004</v>
       </c>
       <c r="B93" s="1">
-        <v>1669.933</v>
+        <v>1693.123</v>
       </c>
       <c r="C93" s="1">
-        <v>2999.5</v>
+        <v>2999.6</v>
       </c>
       <c r="D93" s="1">
-        <v>-13.95</v>
+        <v>-14.05</v>
       </c>
       <c r="E93" s="1"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
-        <v>792.76900000000001</v>
+        <v>878.39599999999996</v>
       </c>
       <c r="B94" s="1">
-        <v>1573.203</v>
+        <v>1592.34</v>
       </c>
       <c r="C94" s="1">
-        <v>2999.5</v>
+        <v>2999.6</v>
       </c>
       <c r="D94" s="1">
-        <v>-11.92</v>
+        <v>-12</v>
       </c>
       <c r="E94" s="1"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
-        <v>789.74400000000003</v>
+        <v>873.47900000000004</v>
       </c>
       <c r="B95" s="1">
-        <v>1479.0119999999999</v>
+        <v>1495.0229999999999</v>
       </c>
       <c r="C95" s="1">
-        <v>2999.5</v>
+        <v>2999.6</v>
       </c>
       <c r="D95" s="1">
-        <v>-9.92</v>
+        <v>-9.98</v>
       </c>
       <c r="E95" s="1"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
-        <v>787.23</v>
+        <v>869.44100000000003</v>
       </c>
       <c r="B96" s="1">
-        <v>1385.643</v>
+        <v>1399.277</v>
       </c>
       <c r="C96" s="1">
-        <v>2999.5</v>
+        <v>2999.6</v>
       </c>
       <c r="D96" s="1">
-        <v>-7.92</v>
+        <v>-8.08</v>
       </c>
       <c r="E96" s="1"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
-        <v>785.18100000000004</v>
+        <v>865.69600000000003</v>
       </c>
       <c r="B97" s="1">
-        <v>1292.396</v>
+        <v>1300.4359999999999</v>
       </c>
       <c r="C97" s="1">
-        <v>2999.5</v>
+        <v>2999.6</v>
       </c>
       <c r="D97" s="1">
-        <v>-5.92</v>
+        <v>-6</v>
       </c>
       <c r="E97" s="1"/>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
-        <v>783.75599999999997</v>
+        <v>862.99</v>
       </c>
       <c r="B98" s="1">
-        <v>1201.1769999999999</v>
+        <v>1205.2550000000001</v>
       </c>
       <c r="C98" s="1">
-        <v>2999.5</v>
+        <v>2999.6</v>
       </c>
       <c r="D98" s="1">
-        <v>-3.95</v>
+        <v>-3.98</v>
       </c>
       <c r="E98" s="1"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
-        <v>782.58600000000001</v>
+        <v>860.90499999999997</v>
       </c>
       <c r="B99" s="1">
-        <v>1108.0160000000001</v>
+        <v>1112.248</v>
       </c>
       <c r="C99" s="1">
-        <v>2999.5</v>
+        <v>2999.6</v>
       </c>
       <c r="D99" s="1">
-        <v>-1.92</v>
+        <v>-2</v>
       </c>
       <c r="E99" s="1"/>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
-        <v>782.34</v>
+        <v>859.33900000000006</v>
       </c>
       <c r="B100" s="1">
-        <v>1016.774</v>
+        <v>1017.742</v>
       </c>
       <c r="C100" s="1">
-        <v>2999.5</v>
+        <v>2999.6</v>
       </c>
       <c r="D100" s="1">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="E100" s="1"/>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
-        <v>782.05200000000002</v>
+        <v>858.48199999999997</v>
       </c>
       <c r="B101" s="1">
-        <v>923.55200000000002</v>
+        <v>924.80200000000002</v>
       </c>
       <c r="C101" s="1">
-        <v>2999.5</v>
+        <v>2999.6</v>
       </c>
       <c r="D101" s="1">
-        <v>2.0499999999999998</v>
+        <v>2.02</v>
       </c>
       <c r="E101" s="1"/>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
-        <v>782.68799999999999</v>
+        <v>858.32</v>
       </c>
       <c r="B102" s="1">
-        <v>830.93</v>
+        <v>831.57</v>
       </c>
       <c r="C102" s="1">
-        <v>2999.5</v>
+        <v>2999.6</v>
       </c>
       <c r="D102" s="1">
-        <v>4.05</v>
+        <v>4.0199999999999996</v>
       </c>
       <c r="E102" s="1"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
-        <v>783.84900000000005</v>
+        <v>858.63199999999995</v>
       </c>
       <c r="B103" s="1">
-        <v>737.09799999999996</v>
+        <v>738.298</v>
       </c>
       <c r="C103" s="1">
-        <v>2999.5</v>
+        <v>2999.6</v>
       </c>
       <c r="D103" s="1">
-        <v>6.05</v>
+        <v>6</v>
       </c>
       <c r="E103" s="1"/>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
-        <v>785.33199999999999</v>
+        <v>859.79200000000003</v>
       </c>
       <c r="B104" s="1">
-        <v>643.83699999999999</v>
+        <v>642.49400000000003</v>
       </c>
       <c r="C104" s="1">
-        <v>2999.5</v>
+        <v>2999.6</v>
       </c>
       <c r="D104" s="1">
-        <v>8.0500000000000007</v>
+        <v>8.07</v>
       </c>
       <c r="E104" s="1"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
-        <v>787.50099999999998</v>
+        <v>861.39800000000002</v>
       </c>
       <c r="B105" s="1">
-        <v>549.30499999999995</v>
+        <v>550.26900000000001</v>
       </c>
       <c r="C105" s="1">
-        <v>2999.5</v>
+        <v>2999.6</v>
       </c>
       <c r="D105" s="1">
-        <v>10.02</v>
+        <v>10</v>
       </c>
       <c r="E105" s="1"/>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
-        <v>789.76800000000003</v>
+        <v>863.80100000000004</v>
       </c>
       <c r="B106" s="1">
-        <v>451.07900000000001</v>
+        <v>452.92399999999998</v>
       </c>
       <c r="C106" s="1">
-        <v>2999.5</v>
+        <v>2999.6</v>
       </c>
       <c r="D106" s="1">
-        <v>12.02</v>
+        <v>12.05</v>
       </c>
       <c r="E106" s="1"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
-        <v>792.88599999999997</v>
+        <v>866.55799999999999</v>
       </c>
       <c r="B107" s="1">
-        <v>353.61900000000003</v>
+        <v>356.90300000000002</v>
       </c>
       <c r="C107" s="1">
-        <v>2999.5</v>
+        <v>2999.6</v>
       </c>
       <c r="D107" s="1">
-        <v>14.08</v>
+        <v>14.02</v>
       </c>
       <c r="E107" s="1"/>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="1">
-        <v>796.101</v>
+        <v>869.99</v>
       </c>
       <c r="B108" s="1">
-        <v>257.32400000000001</v>
+        <v>258.178</v>
       </c>
       <c r="C108" s="1">
-        <v>2999.5</v>
+        <v>2999.6</v>
       </c>
       <c r="D108" s="1">
-        <v>16.05</v>
+        <v>16.02</v>
       </c>
       <c r="E108" s="1"/>
     </row>

</xml_diff>

<commit_message>
ErrorDetecter and PredictSA function added
</commit_message>
<xml_diff>
--- a/Cam2calib.xlsx
+++ b/Cam2calib.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DE68FD9-6BF4-4AC1-BBB2-BC45FDB76975}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C09182-A1C1-43A9-848A-61895008525F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13131" yWindow="4500" windowWidth="17718" windowHeight="13226" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34037" yWindow="4269" windowWidth="29246" windowHeight="12737" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -352,13 +352,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1">
-        <v>940.52800000000002</v>
+        <v>884.899</v>
       </c>
       <c r="B1" s="1">
-        <v>1019.168</v>
+        <v>1019.2619999999999</v>
       </c>
       <c r="C1" s="1">
-        <v>2501.1999999999998</v>
+        <v>2499.9</v>
       </c>
       <c r="D1" s="1">
         <v>0</v>
@@ -367,193 +367,193 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>974.19399999999996</v>
+        <v>890.87699999999995</v>
       </c>
       <c r="B2" s="1">
-        <v>1793.377</v>
+        <v>1792.6510000000001</v>
       </c>
       <c r="C2" s="1">
-        <v>2501.1999999999998</v>
+        <v>2499.9</v>
       </c>
       <c r="D2" s="1">
-        <v>-15.93</v>
+        <v>-16.07</v>
       </c>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <v>967.72199999999998</v>
+        <v>887.62300000000005</v>
       </c>
       <c r="B3" s="1">
-        <v>1697.279</v>
+        <v>1687.116</v>
       </c>
       <c r="C3" s="1">
-        <v>2501.1999999999998</v>
+        <v>2499.9</v>
       </c>
       <c r="D3" s="1">
-        <v>-14.02</v>
+        <v>-13.97</v>
       </c>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>961.42200000000003</v>
+        <v>885.60299999999995</v>
       </c>
       <c r="B4" s="1">
-        <v>1597.1289999999999</v>
+        <v>1588.471</v>
       </c>
       <c r="C4" s="1">
-        <v>2501.1999999999998</v>
+        <v>2499.9</v>
       </c>
       <c r="D4" s="1">
-        <v>-12</v>
+        <v>-11.95</v>
       </c>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
-        <v>956.20899999999995</v>
+        <v>883.98599999999999</v>
       </c>
       <c r="B5" s="1">
-        <v>1499.7429999999999</v>
+        <v>1491.7560000000001</v>
       </c>
       <c r="C5" s="1">
-        <v>2501.1999999999998</v>
+        <v>2499.9</v>
       </c>
       <c r="D5" s="1">
-        <v>-10</v>
+        <v>-10.050000000000001</v>
       </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
-        <v>951.48400000000004</v>
+        <v>882.92499999999995</v>
       </c>
       <c r="B6" s="1">
-        <v>1401.5150000000001</v>
+        <v>1391.942</v>
       </c>
       <c r="C6" s="1">
-        <v>2501.1999999999998</v>
+        <v>2499.9</v>
       </c>
       <c r="D6" s="1">
-        <v>-8.1</v>
+        <v>-7.97</v>
       </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
-        <v>947.452</v>
+        <v>882.52599999999995</v>
       </c>
       <c r="B7" s="1">
-        <v>1301.2070000000001</v>
+        <v>1295.702</v>
       </c>
       <c r="C7" s="1">
-        <v>2501.1999999999998</v>
+        <v>2499.9</v>
       </c>
       <c r="D7" s="1">
-        <v>-6</v>
+        <v>-5.95</v>
       </c>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
-        <v>944.45699999999999</v>
+        <v>882.51400000000001</v>
       </c>
       <c r="B8" s="1">
-        <v>1206.1579999999999</v>
+        <v>1202.796</v>
       </c>
       <c r="C8" s="1">
-        <v>2501.1999999999998</v>
+        <v>2499.9</v>
       </c>
       <c r="D8" s="1">
-        <v>-3.97</v>
+        <v>-3.95</v>
       </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
-        <v>942.28700000000003</v>
+        <v>883.48900000000003</v>
       </c>
       <c r="B9" s="1">
-        <v>1112.0640000000001</v>
+        <v>1108.885</v>
       </c>
       <c r="C9" s="1">
-        <v>2501.1999999999998</v>
+        <v>2499.9</v>
       </c>
       <c r="D9" s="1">
-        <v>-2</v>
+        <v>-1.95</v>
       </c>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
-        <v>940.51099999999997</v>
+        <v>884.947</v>
       </c>
       <c r="B10" s="1">
-        <v>1016.948</v>
+        <v>1015.559</v>
       </c>
       <c r="C10" s="1">
-        <v>2501.1999999999998</v>
+        <v>2499.9</v>
       </c>
       <c r="D10" s="1">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
-        <v>939.65800000000002</v>
+        <v>886.90599999999995</v>
       </c>
       <c r="B11" s="1">
-        <v>924.05899999999997</v>
+        <v>923.279</v>
       </c>
       <c r="C11" s="1">
-        <v>2501.1999999999998</v>
+        <v>2499.9</v>
       </c>
       <c r="D11" s="1">
-        <v>2.0299999999999998</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
-        <v>939.59199999999998</v>
+        <v>889.471</v>
       </c>
       <c r="B12" s="1">
-        <v>830.86</v>
+        <v>831.21799999999996</v>
       </c>
       <c r="C12" s="1">
-        <v>2501.1999999999998</v>
+        <v>2499.9</v>
       </c>
       <c r="D12" s="1">
-        <v>4.03</v>
+        <v>4.05</v>
       </c>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
-        <v>940.21299999999997</v>
+        <v>892.64200000000005</v>
       </c>
       <c r="B13" s="1">
-        <v>736.54700000000003</v>
+        <v>738.18700000000001</v>
       </c>
       <c r="C13" s="1">
-        <v>2501.1999999999998</v>
+        <v>2499.9</v>
       </c>
       <c r="D13" s="1">
-        <v>6</v>
+        <v>6.05</v>
       </c>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
-        <v>941.851</v>
+        <v>896.53700000000003</v>
       </c>
       <c r="B14" s="1">
-        <v>640.47199999999998</v>
+        <v>644.452</v>
       </c>
       <c r="C14" s="1">
-        <v>2501.1999999999998</v>
+        <v>2499.9</v>
       </c>
       <c r="D14" s="1">
         <v>8.0500000000000007</v>
@@ -562,58 +562,58 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
-        <v>943.67600000000004</v>
+        <v>900.95399999999995</v>
       </c>
       <c r="B15" s="1">
-        <v>546.49800000000005</v>
+        <v>549.80100000000004</v>
       </c>
       <c r="C15" s="1">
-        <v>2501.1999999999998</v>
+        <v>2499.9</v>
       </c>
       <c r="D15" s="1">
-        <v>10.029999999999999</v>
+        <v>10.02</v>
       </c>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
-        <v>946.59100000000001</v>
+        <v>906.26199999999994</v>
       </c>
       <c r="B16" s="1">
-        <v>449.82400000000001</v>
+        <v>452.37200000000001</v>
       </c>
       <c r="C16" s="1">
-        <v>2501.1999999999998</v>
+        <v>2499.9</v>
       </c>
       <c r="D16" s="1">
-        <v>12.03</v>
+        <v>12.05</v>
       </c>
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
-        <v>950.077</v>
+        <v>911.75800000000004</v>
       </c>
       <c r="B17" s="1">
-        <v>351.76299999999998</v>
+        <v>356.05700000000002</v>
       </c>
       <c r="C17" s="1">
-        <v>2501.1999999999998</v>
+        <v>2499.9</v>
       </c>
       <c r="D17" s="1">
-        <v>14.03</v>
+        <v>14.05</v>
       </c>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
-        <v>954.23299999999995</v>
+        <v>917.952</v>
       </c>
       <c r="B18" s="1">
-        <v>252.71100000000001</v>
+        <v>258.08300000000003</v>
       </c>
       <c r="C18" s="1">
-        <v>2501.1999999999998</v>
+        <v>2499.9</v>
       </c>
       <c r="D18" s="1">
         <v>16.02</v>
@@ -622,13 +622,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
-        <v>921.74400000000003</v>
+        <v>865.96</v>
       </c>
       <c r="B19" s="1">
-        <v>1019.15</v>
+        <v>1019.212</v>
       </c>
       <c r="C19" s="1">
-        <v>2600.9</v>
+        <v>2599.6</v>
       </c>
       <c r="D19" s="1">
         <v>0</v>
@@ -637,208 +637,208 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
-        <v>954.76099999999997</v>
+        <v>871.01700000000005</v>
       </c>
       <c r="B20" s="1">
-        <v>1792.7629999999999</v>
+        <v>1791.6890000000001</v>
       </c>
       <c r="C20" s="1">
-        <v>2600.9</v>
+        <v>2599.6</v>
       </c>
       <c r="D20" s="1">
-        <v>-15.92</v>
+        <v>-16.07</v>
       </c>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
-        <v>948.12699999999995</v>
+        <v>868.37099999999998</v>
       </c>
       <c r="B21" s="1">
-        <v>1695.704</v>
+        <v>1685.865</v>
       </c>
       <c r="C21" s="1">
-        <v>2600.9</v>
+        <v>2599.6</v>
       </c>
       <c r="D21" s="1">
-        <v>-14.05</v>
+        <v>-13.97</v>
       </c>
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
-        <v>942.23</v>
+        <v>866.20699999999999</v>
       </c>
       <c r="B22" s="1">
-        <v>1595.482</v>
+        <v>1587.5239999999999</v>
       </c>
       <c r="C22" s="1">
-        <v>2600.9</v>
+        <v>2599.6</v>
       </c>
       <c r="D22" s="1">
-        <v>-12</v>
+        <v>-11.95</v>
       </c>
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
-        <v>937.00400000000002</v>
+        <v>864.851</v>
       </c>
       <c r="B23" s="1">
-        <v>1497.596</v>
+        <v>1490.8679999999999</v>
       </c>
       <c r="C23" s="1">
-        <v>2600.9</v>
+        <v>2599.6</v>
       </c>
       <c r="D23" s="1">
-        <v>-9.9700000000000006</v>
+        <v>-10.050000000000001</v>
       </c>
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
-        <v>932.47</v>
+        <v>863.79700000000003</v>
       </c>
       <c r="B24" s="1">
-        <v>1402.145</v>
+        <v>1391.2840000000001</v>
       </c>
       <c r="C24" s="1">
-        <v>2600.9</v>
+        <v>2599.6</v>
       </c>
       <c r="D24" s="1">
-        <v>-8.1</v>
+        <v>-7.97</v>
       </c>
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
-        <v>928.51300000000003</v>
+        <v>863.47900000000004</v>
       </c>
       <c r="B25" s="1">
-        <v>1302.3710000000001</v>
+        <v>1295.44</v>
       </c>
       <c r="C25" s="1">
-        <v>2600.9</v>
+        <v>2599.6</v>
       </c>
       <c r="D25" s="1">
-        <v>-6</v>
+        <v>-5.95</v>
       </c>
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
-        <v>925.53200000000004</v>
+        <v>863.56</v>
       </c>
       <c r="B26" s="1">
-        <v>1206.7349999999999</v>
+        <v>1202.1010000000001</v>
       </c>
       <c r="C26" s="1">
-        <v>2600.9</v>
+        <v>2599.6</v>
       </c>
       <c r="D26" s="1">
-        <v>-4</v>
+        <v>-3.95</v>
       </c>
       <c r="E26" s="1"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
-        <v>923.25400000000002</v>
+        <v>864.54700000000003</v>
       </c>
       <c r="B27" s="1">
-        <v>1111.289</v>
+        <v>1108.6669999999999</v>
       </c>
       <c r="C27" s="1">
-        <v>2600.9</v>
+        <v>2599.6</v>
       </c>
       <c r="D27" s="1">
-        <v>-2</v>
+        <v>-1.95</v>
       </c>
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
-        <v>921.66</v>
+        <v>865.98699999999997</v>
       </c>
       <c r="B28" s="1">
-        <v>1017.107</v>
+        <v>1016.287</v>
       </c>
       <c r="C28" s="1">
-        <v>2600.9</v>
+        <v>2599.6</v>
       </c>
       <c r="D28" s="1">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="E28" s="1"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
-        <v>920.87699999999995</v>
+        <v>867.976</v>
       </c>
       <c r="B29" s="1">
-        <v>924.04600000000005</v>
+        <v>922.98699999999997</v>
       </c>
       <c r="C29" s="1">
-        <v>2600.9</v>
+        <v>2599.6</v>
       </c>
       <c r="D29" s="1">
-        <v>2.0299999999999998</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
-        <v>920.64099999999996</v>
+        <v>870.43</v>
       </c>
       <c r="B30" s="1">
-        <v>830.97299999999996</v>
+        <v>831.56200000000001</v>
       </c>
       <c r="C30" s="1">
-        <v>2600.9</v>
+        <v>2599.6</v>
       </c>
       <c r="D30" s="1">
-        <v>4.03</v>
+        <v>4.05</v>
       </c>
       <c r="E30" s="1"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
-        <v>921.43899999999996</v>
+        <v>873.63599999999997</v>
       </c>
       <c r="B31" s="1">
-        <v>736.85799999999995</v>
+        <v>738.58500000000004</v>
       </c>
       <c r="C31" s="1">
-        <v>2600.9</v>
+        <v>2599.6</v>
       </c>
       <c r="D31" s="1">
-        <v>6.03</v>
+        <v>6.05</v>
       </c>
       <c r="E31" s="1"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
-        <v>922.85500000000002</v>
+        <v>877.48500000000001</v>
       </c>
       <c r="B32" s="1">
-        <v>642.21</v>
+        <v>644.26800000000003</v>
       </c>
       <c r="C32" s="1">
-        <v>2600.9</v>
+        <v>2599.6</v>
       </c>
       <c r="D32" s="1">
-        <v>8.0299999999999994</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="E32" s="1"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
-        <v>924.68299999999999</v>
+        <v>881.74400000000003</v>
       </c>
       <c r="B33" s="1">
-        <v>546.38599999999997</v>
+        <v>550.01800000000003</v>
       </c>
       <c r="C33" s="1">
-        <v>2600.9</v>
+        <v>2599.6</v>
       </c>
       <c r="D33" s="1">
         <v>10.050000000000001</v>
@@ -847,58 +847,58 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
-        <v>927.43700000000001</v>
+        <v>886.64599999999996</v>
       </c>
       <c r="B34" s="1">
-        <v>451.21199999999999</v>
+        <v>454.19200000000001</v>
       </c>
       <c r="C34" s="1">
-        <v>2600.9</v>
+        <v>2599.6</v>
       </c>
       <c r="D34" s="1">
-        <v>12.03</v>
+        <v>12.02</v>
       </c>
       <c r="E34" s="1"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
-        <v>930.73299999999995</v>
+        <v>892.15499999999997</v>
       </c>
       <c r="B35" s="1">
-        <v>354.00400000000002</v>
+        <v>356.55599999999998</v>
       </c>
       <c r="C35" s="1">
-        <v>2600.9</v>
+        <v>2599.6</v>
       </c>
       <c r="D35" s="1">
-        <v>14.03</v>
+        <v>14.05</v>
       </c>
       <c r="E35" s="1"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
-        <v>934.56200000000001</v>
+        <v>898.33100000000002</v>
       </c>
       <c r="B36" s="1">
-        <v>255.38300000000001</v>
+        <v>258.57499999999999</v>
       </c>
       <c r="C36" s="1">
-        <v>2600.9</v>
+        <v>2599.6</v>
       </c>
       <c r="D36" s="1">
-        <v>16.03</v>
+        <v>16.02</v>
       </c>
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
-        <v>904.43299999999999</v>
+        <v>848.35699999999997</v>
       </c>
       <c r="B37" s="1">
-        <v>1019.401</v>
+        <v>1019.653</v>
       </c>
       <c r="C37" s="1">
-        <v>2700.6</v>
+        <v>2699.3</v>
       </c>
       <c r="D37" s="1">
         <v>0</v>
@@ -907,238 +907,238 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
-        <v>936.63099999999997</v>
+        <v>852.70399999999995</v>
       </c>
       <c r="B38" s="1">
-        <v>1792.771</v>
+        <v>1790.65</v>
       </c>
       <c r="C38" s="1">
-        <v>2700.6</v>
+        <v>2699.3</v>
       </c>
       <c r="D38" s="1">
-        <v>-15.95</v>
+        <v>-16.07</v>
       </c>
       <c r="E38" s="1"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
-        <v>930.48500000000001</v>
+        <v>850.404</v>
       </c>
       <c r="B39" s="1">
-        <v>1695.617</v>
+        <v>1685.2550000000001</v>
       </c>
       <c r="C39" s="1">
-        <v>2700.6</v>
+        <v>2699.3</v>
       </c>
       <c r="D39" s="1">
-        <v>-14.05</v>
+        <v>-13.97</v>
       </c>
       <c r="E39" s="1"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
-        <v>924.43299999999999</v>
+        <v>848.399</v>
       </c>
       <c r="B40" s="1">
-        <v>1594.096</v>
+        <v>1587.15</v>
       </c>
       <c r="C40" s="1">
-        <v>2700.6</v>
+        <v>2699.3</v>
       </c>
       <c r="D40" s="1">
-        <v>-12</v>
+        <v>-11.93</v>
       </c>
       <c r="E40" s="1"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
-        <v>919.33299999999997</v>
+        <v>846.90700000000004</v>
       </c>
       <c r="B41" s="1">
-        <v>1496.7840000000001</v>
+        <v>1492.0419999999999</v>
       </c>
       <c r="C41" s="1">
-        <v>2700.6</v>
+        <v>2699.3</v>
       </c>
       <c r="D41" s="1">
-        <v>-9.9700000000000006</v>
+        <v>-10.07</v>
       </c>
       <c r="E41" s="1"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
-        <v>915.077</v>
+        <v>846.07799999999997</v>
       </c>
       <c r="B42" s="1">
-        <v>1401.502</v>
+        <v>1391.395</v>
       </c>
       <c r="C42" s="1">
-        <v>2700.6</v>
+        <v>2699.3</v>
       </c>
       <c r="D42" s="1">
-        <v>-8.1</v>
+        <v>-7.95</v>
       </c>
       <c r="E42" s="1"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
-        <v>911.01300000000003</v>
+        <v>845.59500000000003</v>
       </c>
       <c r="B43" s="1">
-        <v>1301.3430000000001</v>
+        <v>1296.5219999999999</v>
       </c>
       <c r="C43" s="1">
-        <v>2700.6</v>
+        <v>2699.3</v>
       </c>
       <c r="D43" s="1">
-        <v>-6</v>
+        <v>-5.97</v>
       </c>
       <c r="E43" s="1"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
-        <v>908.22299999999996</v>
+        <v>846.03599999999994</v>
       </c>
       <c r="B44" s="1">
-        <v>1206.2529999999999</v>
+        <v>1201.866</v>
       </c>
       <c r="C44" s="1">
-        <v>2700.6</v>
+        <v>2699.3</v>
       </c>
       <c r="D44" s="1">
-        <v>-4</v>
+        <v>-3.95</v>
       </c>
       <c r="E44" s="1"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
-        <v>905.84799999999996</v>
+        <v>846.96500000000003</v>
       </c>
       <c r="B45" s="1">
-        <v>1111.221</v>
+        <v>1109.7809999999999</v>
       </c>
       <c r="C45" s="1">
-        <v>2700.6</v>
+        <v>2699.3</v>
       </c>
       <c r="D45" s="1">
-        <v>-2</v>
+        <v>-1.95</v>
       </c>
       <c r="E45" s="1"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
-        <v>904.39200000000005</v>
+        <v>848.447</v>
       </c>
       <c r="B46" s="1">
-        <v>1016.737</v>
+        <v>1015.826</v>
       </c>
       <c r="C46" s="1">
-        <v>2700.6</v>
+        <v>2699.3</v>
       </c>
       <c r="D46" s="1">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="E46" s="1"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
-        <v>903.42200000000003</v>
+        <v>850.52099999999996</v>
       </c>
       <c r="B47" s="1">
-        <v>923.51800000000003</v>
+        <v>923.28599999999994</v>
       </c>
       <c r="C47" s="1">
-        <v>2700.6</v>
+        <v>2699.3</v>
       </c>
       <c r="D47" s="1">
-        <v>2.0299999999999998</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="E47" s="1"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
-        <v>903.43499999999995</v>
+        <v>852.96699999999998</v>
       </c>
       <c r="B48" s="1">
-        <v>830.33399999999995</v>
+        <v>832.17399999999998</v>
       </c>
       <c r="C48" s="1">
-        <v>2700.6</v>
+        <v>2699.3</v>
       </c>
       <c r="D48" s="1">
-        <v>4.03</v>
+        <v>4.05</v>
       </c>
       <c r="E48" s="1"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
-        <v>903.846</v>
+        <v>856.03800000000001</v>
       </c>
       <c r="B49" s="1">
-        <v>736.50599999999997</v>
+        <v>739.37699999999995</v>
       </c>
       <c r="C49" s="1">
-        <v>2700.6</v>
+        <v>2699.3</v>
       </c>
       <c r="D49" s="1">
-        <v>6.03</v>
+        <v>6.05</v>
       </c>
       <c r="E49" s="1"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
-        <v>905.08500000000004</v>
+        <v>859.71299999999997</v>
       </c>
       <c r="B50" s="1">
-        <v>642.03499999999997</v>
+        <v>645.24199999999996</v>
       </c>
       <c r="C50" s="1">
-        <v>2700.6</v>
+        <v>2699.3</v>
       </c>
       <c r="D50" s="1">
-        <v>8.0299999999999994</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="E50" s="1"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
-        <v>906.95500000000004</v>
+        <v>864.22199999999998</v>
       </c>
       <c r="B51" s="1">
-        <v>547.07600000000002</v>
+        <v>551.02800000000002</v>
       </c>
       <c r="C51" s="1">
-        <v>2700.6</v>
+        <v>2699.3</v>
       </c>
       <c r="D51" s="1">
-        <v>10.029999999999999</v>
+        <v>10.050000000000001</v>
       </c>
       <c r="E51" s="1"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
-        <v>909.62099999999998</v>
+        <v>868.72</v>
       </c>
       <c r="B52" s="1">
-        <v>450.85199999999998</v>
+        <v>454.75700000000001</v>
       </c>
       <c r="C52" s="1">
-        <v>2700.6</v>
+        <v>2699.3</v>
       </c>
       <c r="D52" s="1">
-        <v>12.03</v>
+        <v>12.02</v>
       </c>
       <c r="E52" s="1"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
-        <v>912.94600000000003</v>
+        <v>874.32399999999996</v>
       </c>
       <c r="B53" s="1">
-        <v>352.90800000000002</v>
+        <v>357.36799999999999</v>
       </c>
       <c r="C53" s="1">
-        <v>2700.6</v>
+        <v>2699.3</v>
       </c>
       <c r="D53" s="1">
         <v>14.05</v>
@@ -1147,28 +1147,28 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
-        <v>916.55</v>
+        <v>880.24699999999996</v>
       </c>
       <c r="B54" s="1">
-        <v>255.81200000000001</v>
+        <v>260.10300000000001</v>
       </c>
       <c r="C54" s="1">
-        <v>2700.6</v>
+        <v>2699.3</v>
       </c>
       <c r="D54" s="1">
-        <v>16.03</v>
+        <v>16.02</v>
       </c>
       <c r="E54" s="1"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
-        <v>888.32</v>
+        <v>831.99800000000005</v>
       </c>
       <c r="B55" s="1">
-        <v>1019.26</v>
+        <v>1019.19</v>
       </c>
       <c r="C55" s="1">
-        <v>2800.3</v>
+        <v>2799</v>
       </c>
       <c r="D55" s="1">
         <v>0</v>
@@ -1177,163 +1177,163 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
-        <v>919.83799999999997</v>
+        <v>835.74199999999996</v>
       </c>
       <c r="B56" s="1">
-        <v>1791.778</v>
+        <v>1790.6859999999999</v>
       </c>
       <c r="C56" s="1">
-        <v>2800.3</v>
+        <v>2799</v>
       </c>
       <c r="D56" s="1">
-        <v>-15.93</v>
+        <v>-16.07</v>
       </c>
       <c r="E56" s="1"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
-        <v>913.77800000000002</v>
+        <v>833.48400000000004</v>
       </c>
       <c r="B57" s="1">
-        <v>1695.8130000000001</v>
+        <v>1685.38</v>
       </c>
       <c r="C57" s="1">
-        <v>2800.3</v>
+        <v>2799</v>
       </c>
       <c r="D57" s="1">
-        <v>-14.05</v>
+        <v>-13.97</v>
       </c>
       <c r="E57" s="1"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
-        <v>908.02499999999998</v>
+        <v>831.59400000000005</v>
       </c>
       <c r="B58" s="1">
-        <v>1594.627</v>
+        <v>1586.915</v>
       </c>
       <c r="C58" s="1">
-        <v>2800.3</v>
+        <v>2799</v>
       </c>
       <c r="D58" s="1">
-        <v>-12</v>
+        <v>-11.93</v>
       </c>
       <c r="E58" s="1"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
-        <v>902.79</v>
+        <v>830.30100000000004</v>
       </c>
       <c r="B59" s="1">
-        <v>1497.58</v>
+        <v>1491.454</v>
       </c>
       <c r="C59" s="1">
-        <v>2800.3</v>
+        <v>2799</v>
       </c>
       <c r="D59" s="1">
-        <v>-10</v>
+        <v>-10.07</v>
       </c>
       <c r="E59" s="1"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
-        <v>898.53700000000003</v>
+        <v>829.5</v>
       </c>
       <c r="B60" s="1">
-        <v>1400.2639999999999</v>
+        <v>1390.5920000000001</v>
       </c>
       <c r="C60" s="1">
-        <v>2800.3</v>
+        <v>2799</v>
       </c>
       <c r="D60" s="1">
-        <v>-8.08</v>
+        <v>-7.95</v>
       </c>
       <c r="E60" s="1"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
-        <v>894.88800000000003</v>
+        <v>829.48900000000003</v>
       </c>
       <c r="B61" s="1">
-        <v>1302.0530000000001</v>
+        <v>1296.1790000000001</v>
       </c>
       <c r="C61" s="1">
-        <v>2800.3</v>
+        <v>2799</v>
       </c>
       <c r="D61" s="1">
-        <v>-6</v>
+        <v>-5.97</v>
       </c>
       <c r="E61" s="1"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
-        <v>891.98900000000003</v>
+        <v>829.76499999999999</v>
       </c>
       <c r="B62" s="1">
-        <v>1206.4580000000001</v>
+        <v>1202.058</v>
       </c>
       <c r="C62" s="1">
-        <v>2800.3</v>
+        <v>2799</v>
       </c>
       <c r="D62" s="1">
-        <v>-3.98</v>
+        <v>-3.95</v>
       </c>
       <c r="E62" s="1"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
-        <v>889.83199999999999</v>
+        <v>830.91800000000001</v>
       </c>
       <c r="B63" s="1">
-        <v>1113.1990000000001</v>
+        <v>1109.0150000000001</v>
       </c>
       <c r="C63" s="1">
-        <v>2800.3</v>
+        <v>2799</v>
       </c>
       <c r="D63" s="1">
-        <v>-2</v>
+        <v>-1.95</v>
       </c>
       <c r="E63" s="1"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
-        <v>888.29</v>
+        <v>832.04</v>
       </c>
       <c r="B64" s="1">
-        <v>1018.417</v>
+        <v>1016.273</v>
       </c>
       <c r="C64" s="1">
-        <v>2800.3</v>
+        <v>2799</v>
       </c>
       <c r="D64" s="1">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
       <c r="E64" s="1"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
-        <v>887.40300000000002</v>
+        <v>834.04899999999998</v>
       </c>
       <c r="B65" s="1">
-        <v>925.41800000000001</v>
+        <v>923.69299999999998</v>
       </c>
       <c r="C65" s="1">
-        <v>2800.3</v>
+        <v>2799</v>
       </c>
       <c r="D65" s="1">
-        <v>2</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="E65" s="1"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
-        <v>887.17899999999997</v>
+        <v>836.74900000000002</v>
       </c>
       <c r="B66" s="1">
-        <v>830.80399999999997</v>
+        <v>832.52200000000005</v>
       </c>
       <c r="C66" s="1">
-        <v>2800.3</v>
+        <v>2799</v>
       </c>
       <c r="D66" s="1">
         <v>4.05</v>
@@ -1342,28 +1342,28 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
-        <v>887.57500000000005</v>
+        <v>839.947</v>
       </c>
       <c r="B67" s="1">
-        <v>738.06</v>
+        <v>739.62800000000004</v>
       </c>
       <c r="C67" s="1">
-        <v>2800.3</v>
+        <v>2799</v>
       </c>
       <c r="D67" s="1">
-        <v>6</v>
+        <v>6.05</v>
       </c>
       <c r="E67" s="1"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
-        <v>888.85699999999997</v>
+        <v>843.36</v>
       </c>
       <c r="B68" s="1">
-        <v>642.47</v>
+        <v>645.64599999999996</v>
       </c>
       <c r="C68" s="1">
-        <v>2800.3</v>
+        <v>2799</v>
       </c>
       <c r="D68" s="1">
         <v>8.0500000000000007</v>
@@ -1372,58 +1372,58 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
-        <v>890.70799999999997</v>
+        <v>847.60699999999997</v>
       </c>
       <c r="B69" s="1">
-        <v>548.21900000000005</v>
+        <v>552.08199999999999</v>
       </c>
       <c r="C69" s="1">
-        <v>2800.3</v>
+        <v>2799</v>
       </c>
       <c r="D69" s="1">
-        <v>10.02</v>
+        <v>10.050000000000001</v>
       </c>
       <c r="E69" s="1"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
-        <v>893.096</v>
+        <v>852.31899999999996</v>
       </c>
       <c r="B70" s="1">
-        <v>452.70800000000003</v>
+        <v>456.351</v>
       </c>
       <c r="C70" s="1">
-        <v>2800.3</v>
+        <v>2799</v>
       </c>
       <c r="D70" s="1">
-        <v>12.05</v>
+        <v>12.02</v>
       </c>
       <c r="E70" s="1"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
-        <v>896.03599999999994</v>
+        <v>857.55399999999997</v>
       </c>
       <c r="B71" s="1">
-        <v>357.24799999999999</v>
+        <v>359.18299999999999</v>
       </c>
       <c r="C71" s="1">
-        <v>2800.3</v>
+        <v>2799</v>
       </c>
       <c r="D71" s="1">
-        <v>14.02</v>
+        <v>14.05</v>
       </c>
       <c r="E71" s="1"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
-        <v>899.71100000000001</v>
+        <v>863.351</v>
       </c>
       <c r="B72" s="1">
-        <v>257.05200000000002</v>
+        <v>260.67500000000001</v>
       </c>
       <c r="C72" s="1">
-        <v>2800.3</v>
+        <v>2799</v>
       </c>
       <c r="D72" s="1">
         <v>16.02</v>
@@ -1432,13 +1432,13 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
-        <v>873.18700000000001</v>
+        <v>817.00400000000002</v>
       </c>
       <c r="B73" s="1">
-        <v>1019.168</v>
+        <v>1019.602</v>
       </c>
       <c r="C73" s="1">
-        <v>2900</v>
+        <v>2898.7</v>
       </c>
       <c r="D73" s="1">
         <v>0</v>
@@ -1447,163 +1447,163 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
-        <v>904.26800000000003</v>
+        <v>820.36599999999999</v>
       </c>
       <c r="B74" s="1">
-        <v>1790.653</v>
+        <v>1790.0129999999999</v>
       </c>
       <c r="C74" s="1">
-        <v>2900</v>
+        <v>2898.7</v>
       </c>
       <c r="D74" s="1">
-        <v>-15.95</v>
+        <v>-16.07</v>
       </c>
       <c r="E74" s="1"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
-        <v>898.36300000000006</v>
+        <v>817.94500000000005</v>
       </c>
       <c r="B75" s="1">
-        <v>1693.76</v>
+        <v>1685.067</v>
       </c>
       <c r="C75" s="1">
-        <v>2900</v>
+        <v>2898.7</v>
       </c>
       <c r="D75" s="1">
-        <v>-14.03</v>
+        <v>-13.97</v>
       </c>
       <c r="E75" s="1"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
-        <v>892.67600000000004</v>
+        <v>816.47</v>
       </c>
       <c r="B76" s="1">
-        <v>1594.537</v>
+        <v>1586.4380000000001</v>
       </c>
       <c r="C76" s="1">
-        <v>2900</v>
+        <v>2898.7</v>
       </c>
       <c r="D76" s="1">
-        <v>-12</v>
+        <v>-11.93</v>
       </c>
       <c r="E76" s="1"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
-        <v>887.57299999999998</v>
+        <v>815.13900000000001</v>
       </c>
       <c r="B77" s="1">
-        <v>1496.7760000000001</v>
+        <v>1491.6379999999999</v>
       </c>
       <c r="C77" s="1">
-        <v>2900</v>
+        <v>2898.7</v>
       </c>
       <c r="D77" s="1">
-        <v>-10</v>
+        <v>-10.07</v>
       </c>
       <c r="E77" s="1"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
-        <v>883.45799999999997</v>
+        <v>814.49599999999998</v>
       </c>
       <c r="B78" s="1">
-        <v>1400.202</v>
+        <v>1390.14</v>
       </c>
       <c r="C78" s="1">
-        <v>2900</v>
+        <v>2898.7</v>
       </c>
       <c r="D78" s="1">
-        <v>-8.08</v>
+        <v>-7.95</v>
       </c>
       <c r="E78" s="1"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
-        <v>879.74400000000003</v>
+        <v>814.46900000000005</v>
       </c>
       <c r="B79" s="1">
-        <v>1300.7809999999999</v>
+        <v>1296.412</v>
       </c>
       <c r="C79" s="1">
-        <v>2900</v>
+        <v>2898.7</v>
       </c>
       <c r="D79" s="1">
-        <v>-6</v>
+        <v>-5.97</v>
       </c>
       <c r="E79" s="1"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
-        <v>876.99</v>
+        <v>814.99</v>
       </c>
       <c r="B80" s="1">
-        <v>1206.018</v>
+        <v>1202.097</v>
       </c>
       <c r="C80" s="1">
-        <v>2900</v>
+        <v>2898.7</v>
       </c>
       <c r="D80" s="1">
-        <v>-3.98</v>
+        <v>-3.95</v>
       </c>
       <c r="E80" s="1"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
-        <v>874.75300000000004</v>
+        <v>815.98699999999997</v>
       </c>
       <c r="B81" s="1">
-        <v>1112.3969999999999</v>
+        <v>1109.336</v>
       </c>
       <c r="C81" s="1">
-        <v>2900</v>
+        <v>2898.7</v>
       </c>
       <c r="D81" s="1">
-        <v>-2</v>
+        <v>-1.95</v>
       </c>
       <c r="E81" s="1"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
-        <v>873.15</v>
+        <v>817.09799999999996</v>
       </c>
       <c r="B82" s="1">
-        <v>1017.968</v>
+        <v>1016.545</v>
       </c>
       <c r="C82" s="1">
-        <v>2900</v>
+        <v>2898.7</v>
       </c>
       <c r="D82" s="1">
-        <v>0.02</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E82" s="1"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
-        <v>872.42200000000003</v>
+        <v>819.04300000000001</v>
       </c>
       <c r="B83" s="1">
-        <v>924.92100000000005</v>
+        <v>924.66700000000003</v>
       </c>
       <c r="C83" s="1">
-        <v>2900</v>
+        <v>2898.7</v>
       </c>
       <c r="D83" s="1">
-        <v>2</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="E83" s="1"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
-        <v>872.20600000000002</v>
+        <v>821.78200000000004</v>
       </c>
       <c r="B84" s="1">
-        <v>830.75</v>
+        <v>832.67899999999997</v>
       </c>
       <c r="C84" s="1">
-        <v>2900</v>
+        <v>2898.7</v>
       </c>
       <c r="D84" s="1">
         <v>4.05</v>
@@ -1612,28 +1612,28 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
-        <v>872.60400000000004</v>
+        <v>824.79499999999996</v>
       </c>
       <c r="B85" s="1">
-        <v>738.303</v>
+        <v>739.39400000000001</v>
       </c>
       <c r="C85" s="1">
-        <v>2900</v>
+        <v>2898.7</v>
       </c>
       <c r="D85" s="1">
-        <v>6</v>
+        <v>6.05</v>
       </c>
       <c r="E85" s="1"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
-        <v>873.77700000000004</v>
+        <v>828.274</v>
       </c>
       <c r="B86" s="1">
-        <v>642.77800000000002</v>
+        <v>646.52099999999996</v>
       </c>
       <c r="C86" s="1">
-        <v>2900</v>
+        <v>2898.7</v>
       </c>
       <c r="D86" s="1">
         <v>8.0500000000000007</v>
@@ -1642,28 +1642,28 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
-        <v>875.43100000000004</v>
+        <v>832.43</v>
       </c>
       <c r="B87" s="1">
-        <v>548.88699999999994</v>
+        <v>551.71199999999999</v>
       </c>
       <c r="C87" s="1">
-        <v>2900</v>
+        <v>2898.7</v>
       </c>
       <c r="D87" s="1">
-        <v>10.02</v>
+        <v>10.050000000000001</v>
       </c>
       <c r="E87" s="1"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
-        <v>877.86900000000003</v>
+        <v>837.221</v>
       </c>
       <c r="B88" s="1">
-        <v>453.06400000000002</v>
+        <v>456.86799999999999</v>
       </c>
       <c r="C88" s="1">
-        <v>2900</v>
+        <v>2898.7</v>
       </c>
       <c r="D88" s="1">
         <v>12.02</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
-        <v>880.88800000000003</v>
+        <v>842.01700000000005</v>
       </c>
       <c r="B89" s="1">
-        <v>355.887</v>
+        <v>359.97</v>
       </c>
       <c r="C89" s="1">
-        <v>2900</v>
+        <v>2898.7</v>
       </c>
       <c r="D89" s="1">
         <v>14.05</v>
@@ -1687,13 +1687,13 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
-        <v>884.30799999999999</v>
+        <v>847.86</v>
       </c>
       <c r="B90" s="1">
-        <v>257.714</v>
+        <v>262.154</v>
       </c>
       <c r="C90" s="1">
-        <v>2900</v>
+        <v>2898.7</v>
       </c>
       <c r="D90" s="1">
         <v>16.02</v>
@@ -1702,13 +1702,13 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
-        <v>859.31299999999999</v>
+        <v>803.096</v>
       </c>
       <c r="B91" s="1">
-        <v>1019.399</v>
+        <v>1019.6130000000001</v>
       </c>
       <c r="C91" s="1">
-        <v>2999.6</v>
+        <v>2998.3</v>
       </c>
       <c r="D91" s="1">
         <v>0</v>
@@ -1717,253 +1717,253 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
-        <v>889.76400000000001</v>
+        <v>805.57799999999997</v>
       </c>
       <c r="B92" s="1">
-        <v>1789.8979999999999</v>
+        <v>1789.7270000000001</v>
       </c>
       <c r="C92" s="1">
-        <v>2999.6</v>
+        <v>2998.3</v>
       </c>
       <c r="D92" s="1">
-        <v>-15.95</v>
+        <v>-16.07</v>
       </c>
       <c r="E92" s="1"/>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
-        <v>883.90200000000004</v>
+        <v>803.52</v>
       </c>
       <c r="B93" s="1">
-        <v>1693.123</v>
+        <v>1684.5840000000001</v>
       </c>
       <c r="C93" s="1">
-        <v>2999.6</v>
+        <v>2998.3</v>
       </c>
       <c r="D93" s="1">
-        <v>-14.05</v>
+        <v>-13.97</v>
       </c>
       <c r="E93" s="1"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
-        <v>878.39599999999996</v>
+        <v>802.10699999999997</v>
       </c>
       <c r="B94" s="1">
-        <v>1592.34</v>
+        <v>1585.277</v>
       </c>
       <c r="C94" s="1">
-        <v>2999.6</v>
+        <v>2998.3</v>
       </c>
       <c r="D94" s="1">
-        <v>-12</v>
+        <v>-11.95</v>
       </c>
       <c r="E94" s="1"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
-        <v>873.47900000000004</v>
+        <v>801.00300000000004</v>
       </c>
       <c r="B95" s="1">
-        <v>1495.0229999999999</v>
+        <v>1489.624</v>
       </c>
       <c r="C95" s="1">
-        <v>2999.6</v>
+        <v>2998.3</v>
       </c>
       <c r="D95" s="1">
-        <v>-9.98</v>
+        <v>-10.050000000000001</v>
       </c>
       <c r="E95" s="1"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
-        <v>869.44100000000003</v>
+        <v>800.42499999999995</v>
       </c>
       <c r="B96" s="1">
-        <v>1399.277</v>
+        <v>1390.2180000000001</v>
       </c>
       <c r="C96" s="1">
-        <v>2999.6</v>
+        <v>2998.3</v>
       </c>
       <c r="D96" s="1">
-        <v>-8.08</v>
+        <v>-7.97</v>
       </c>
       <c r="E96" s="1"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
-        <v>865.69600000000003</v>
+        <v>800.33500000000004</v>
       </c>
       <c r="B97" s="1">
-        <v>1300.4359999999999</v>
+        <v>1295.989</v>
       </c>
       <c r="C97" s="1">
-        <v>2999.6</v>
+        <v>2998.3</v>
       </c>
       <c r="D97" s="1">
-        <v>-6</v>
+        <v>-5.95</v>
       </c>
       <c r="E97" s="1"/>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
-        <v>862.99</v>
+        <v>800.98299999999995</v>
       </c>
       <c r="B98" s="1">
-        <v>1205.2550000000001</v>
+        <v>1202.2550000000001</v>
       </c>
       <c r="C98" s="1">
-        <v>2999.6</v>
+        <v>2998.3</v>
       </c>
       <c r="D98" s="1">
-        <v>-3.98</v>
+        <v>-3.95</v>
       </c>
       <c r="E98" s="1"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
-        <v>860.90499999999997</v>
+        <v>801.96500000000003</v>
       </c>
       <c r="B99" s="1">
-        <v>1112.248</v>
+        <v>1109.5920000000001</v>
       </c>
       <c r="C99" s="1">
-        <v>2999.6</v>
+        <v>2998.3</v>
       </c>
       <c r="D99" s="1">
-        <v>-2</v>
+        <v>-1.95</v>
       </c>
       <c r="E99" s="1"/>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
-        <v>859.33900000000006</v>
+        <v>803.13</v>
       </c>
       <c r="B100" s="1">
-        <v>1017.742</v>
+        <v>1016.599</v>
       </c>
       <c r="C100" s="1">
-        <v>2999.6</v>
+        <v>2998.3</v>
       </c>
       <c r="D100" s="1">
-        <v>0.02</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E100" s="1"/>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
-        <v>858.48199999999997</v>
+        <v>805.15099999999995</v>
       </c>
       <c r="B101" s="1">
-        <v>924.80200000000002</v>
+        <v>925.95</v>
       </c>
       <c r="C101" s="1">
-        <v>2999.6</v>
+        <v>2998.3</v>
       </c>
       <c r="D101" s="1">
-        <v>2.02</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="E101" s="1"/>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
-        <v>858.32</v>
+        <v>807.85599999999999</v>
       </c>
       <c r="B102" s="1">
-        <v>831.57</v>
+        <v>833.61400000000003</v>
       </c>
       <c r="C102" s="1">
-        <v>2999.6</v>
+        <v>2998.3</v>
       </c>
       <c r="D102" s="1">
-        <v>4.0199999999999996</v>
+        <v>4.05</v>
       </c>
       <c r="E102" s="1"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
-        <v>858.63199999999995</v>
+        <v>810.85699999999997</v>
       </c>
       <c r="B103" s="1">
-        <v>738.298</v>
+        <v>740.346</v>
       </c>
       <c r="C103" s="1">
-        <v>2999.6</v>
+        <v>2998.3</v>
       </c>
       <c r="D103" s="1">
-        <v>6</v>
+        <v>6.05</v>
       </c>
       <c r="E103" s="1"/>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
-        <v>859.79200000000003</v>
+        <v>814.17700000000002</v>
       </c>
       <c r="B104" s="1">
-        <v>642.49400000000003</v>
+        <v>646.88199999999995</v>
       </c>
       <c r="C104" s="1">
-        <v>2999.6</v>
+        <v>2998.3</v>
       </c>
       <c r="D104" s="1">
-        <v>8.07</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="E104" s="1"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
-        <v>861.39800000000002</v>
+        <v>818.41499999999996</v>
       </c>
       <c r="B105" s="1">
-        <v>550.26900000000001</v>
+        <v>552.79300000000001</v>
       </c>
       <c r="C105" s="1">
-        <v>2999.6</v>
+        <v>2998.3</v>
       </c>
       <c r="D105" s="1">
-        <v>10</v>
+        <v>10.050000000000001</v>
       </c>
       <c r="E105" s="1"/>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
-        <v>863.80100000000004</v>
+        <v>822.87900000000002</v>
       </c>
       <c r="B106" s="1">
-        <v>452.92399999999998</v>
+        <v>457.98399999999998</v>
       </c>
       <c r="C106" s="1">
-        <v>2999.6</v>
+        <v>2998.3</v>
       </c>
       <c r="D106" s="1">
-        <v>12.05</v>
+        <v>12.02</v>
       </c>
       <c r="E106" s="1"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
-        <v>866.55799999999999</v>
+        <v>827.81799999999998</v>
       </c>
       <c r="B107" s="1">
-        <v>356.90300000000002</v>
+        <v>360.18900000000002</v>
       </c>
       <c r="C107" s="1">
-        <v>2999.6</v>
+        <v>2998.3</v>
       </c>
       <c r="D107" s="1">
-        <v>14.02</v>
+        <v>14.05</v>
       </c>
       <c r="E107" s="1"/>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="1">
-        <v>869.99</v>
+        <v>833.27099999999996</v>
       </c>
       <c r="B108" s="1">
-        <v>258.178</v>
+        <v>262.98200000000003</v>
       </c>
       <c r="C108" s="1">
-        <v>2999.6</v>
+        <v>2998.3</v>
       </c>
       <c r="D108" s="1">
         <v>16.02</v>

</xml_diff>